<commit_message>
HSI v1.1 , applied suggested modifications Signed-off-by: ahmedRefaat95 <ahmed.refaat.rashad@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/HSI_Review.xlsx
+++ b/Input Documents/HSI_Review.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7122DD7B-D648-44FD-9E2E-2B71B522001A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -116,9 +115,6 @@
     <t xml:space="preserve">Initial creation </t>
   </si>
   <si>
-    <t>Document statuc table : you should put the status of the document which exist in the start in a table , this table holds the following info "Document name , Suther , Version , Auther , Last update Date"</t>
-  </si>
-  <si>
     <t>Page 1</t>
   </si>
   <si>
@@ -156,11 +152,14 @@
     <t xml:space="preserve">Req _ DIGELV _ HSI _03_V1.0 : what is the goal of this req ? 
 If you should say the system Keypad to enter the pass and ID for the input and LCD to display the out put , but here you refere to CYRS req , Why ? ,,, you don't have to </t>
   </si>
+  <si>
+    <t>Document status table : you should put the status of the document which exist in the start in a table , this table holds the following info "Document name , Suther , Version , Auther , Last update Date"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -525,12 +524,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,43 +571,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -916,7 +915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -930,189 +929,206 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="28"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="29"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="39"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="29"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="30">
-        <v>1</v>
-      </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="34"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="31"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1129,23 +1145,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1153,11 +1152,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,22 +1203,22 @@
     </row>
     <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
@@ -1229,22 +1228,22 @@
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="E3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
@@ -1257,22 +1256,22 @@
     </row>
     <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>39</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>40</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
@@ -1285,22 +1284,22 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
@@ -1310,22 +1309,22 @@
     </row>
     <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="E6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
@@ -1812,10 +1811,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>$K$3:$K$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>$K$6:$K$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>